<commit_message>
Updated tests that I previously messed up
</commit_message>
<xml_diff>
--- a/test16-strip/dssim.xlsx
+++ b/test16-strip/dssim.xlsx
@@ -1434,8 +1434,8 @@
   <dimension ref="A1:E134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A112" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:E122"/>
+      <pane ySplit="2" topLeftCell="A109" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1655,13 +1655,13 @@
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="6">
-        <v>1.1604E-2</v>
+        <v>1.1606E-2</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="6">
-        <v>1.1604E-2</v>
+        <v>1.1606E-2</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>149</v>
@@ -1683,13 +1683,13 @@
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="2">
-        <v>4.2764999999999997E-2</v>
+        <v>4.2873000000000001E-2</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D18" s="2">
-        <v>4.2764999999999997E-2</v>
+        <v>4.2873000000000001E-2</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>151</v>
@@ -1711,13 +1711,13 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="2">
-        <v>6.3550000000000004E-3</v>
+        <v>6.3559999999999997E-3</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="2">
-        <v>6.3550000000000004E-3</v>
+        <v>6.3559999999999997E-3</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>153</v>
@@ -1725,13 +1725,13 @@
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="6">
-        <v>1.776E-3</v>
+        <v>1.7780000000000001E-3</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="6">
-        <v>1.776E-3</v>
+        <v>1.7780000000000001E-3</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>154</v>
@@ -1753,13 +1753,13 @@
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="6">
-        <v>5.8380000000000003E-3</v>
+        <v>5.8409999999999998E-3</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="6">
-        <v>5.8380000000000003E-3</v>
+        <v>5.8409999999999998E-3</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>156</v>
@@ -1767,13 +1767,13 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="6">
-        <v>2.9009999999999999E-3</v>
+        <v>2.9020000000000001E-3</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="6">
-        <v>2.9009999999999999E-3</v>
+        <v>2.9020000000000001E-3</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>157</v>
@@ -1795,13 +1795,13 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="6">
-        <v>3.9579999999999997E-3</v>
+        <v>3.9529999999999999E-3</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="6">
-        <v>3.9579999999999997E-3</v>
+        <v>3.9529999999999999E-3</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>159</v>
@@ -1809,13 +1809,13 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="2">
-        <v>1.2260000000000001E-3</v>
+        <v>1.225E-3</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="2">
-        <v>1.2260000000000001E-3</v>
+        <v>1.225E-3</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>160</v>
@@ -1823,13 +1823,13 @@
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2">
-        <v>3.0609999999999999E-3</v>
+        <v>3.088E-3</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="2">
-        <v>3.0609999999999999E-3</v>
+        <v>3.088E-3</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>161</v>
@@ -1837,13 +1837,13 @@
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="2">
-        <v>6.1419999999999999E-3</v>
+        <v>6.1970000000000003E-3</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="2">
-        <v>6.1419999999999999E-3</v>
+        <v>6.1970000000000003E-3</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>162</v>
@@ -1851,13 +1851,13 @@
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="2">
-        <v>4.3999999999999999E-5</v>
+        <v>4.6E-5</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D30" s="2">
-        <v>4.3999999999999999E-5</v>
+        <v>4.6E-5</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>163</v>
@@ -1879,13 +1879,13 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="2">
-        <v>9.6699999999999998E-4</v>
+        <v>9.6599999999999995E-4</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="2">
-        <v>9.6699999999999998E-4</v>
+        <v>9.6599999999999995E-4</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>165</v>
@@ -1921,13 +1921,13 @@
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2">
-        <v>2.7712000000000001E-2</v>
+        <v>2.6932999999999999E-2</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D35" s="2">
-        <v>2.7712000000000001E-2</v>
+        <v>2.6932999999999999E-2</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>168</v>
@@ -1991,13 +1991,13 @@
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="2">
-        <v>1.4735E-2</v>
+        <v>1.4736000000000001E-2</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>53</v>
       </c>
       <c r="D40" s="2">
-        <v>1.4735E-2</v>
+        <v>1.4736000000000001E-2</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>173</v>
@@ -2033,13 +2033,13 @@
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="2">
-        <v>4.5900000000000003E-3</v>
+        <v>4.5880000000000001E-3</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="2">
-        <v>4.5900000000000003E-3</v>
+        <v>4.5880000000000001E-3</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>176</v>
@@ -2131,13 +2131,13 @@
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="6">
-        <v>8.8889999999999993E-3</v>
+        <v>8.9289999999999994E-3</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>63</v>
       </c>
       <c r="D50" s="6">
-        <v>8.8889999999999993E-3</v>
+        <v>8.9289999999999994E-3</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>183</v>
@@ -2145,13 +2145,13 @@
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="6">
-        <v>3.9370000000000004E-3</v>
+        <v>3.9389999999999998E-3</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>64</v>
       </c>
       <c r="D51" s="6">
-        <v>3.9370000000000004E-3</v>
+        <v>3.9389999999999998E-3</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>184</v>
@@ -2201,13 +2201,13 @@
     </row>
     <row r="55" spans="2:5">
       <c r="B55" s="6">
-        <v>6.9540000000000001E-3</v>
+        <v>6.953E-3</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>68</v>
       </c>
       <c r="D55" s="6">
-        <v>6.9540000000000001E-3</v>
+        <v>6.953E-3</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>188</v>
@@ -2257,13 +2257,13 @@
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="6">
-        <v>5.04E-4</v>
+        <v>5.0500000000000002E-4</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D59" s="6">
-        <v>5.04E-4</v>
+        <v>5.0500000000000002E-4</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>192</v>
@@ -2271,13 +2271,13 @@
     </row>
     <row r="60" spans="2:5">
       <c r="B60" s="6">
-        <v>1.016E-3</v>
+        <v>1.0269999999999999E-3</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D60" s="6">
-        <v>1.016E-3</v>
+        <v>1.0269999999999999E-3</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>193</v>
@@ -2299,13 +2299,13 @@
     </row>
     <row r="62" spans="2:5">
       <c r="B62" s="6">
-        <v>2.238E-3</v>
+        <v>2.2399999999999998E-3</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>75</v>
       </c>
       <c r="D62" s="6">
-        <v>2.238E-3</v>
+        <v>2.2399999999999998E-3</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>195</v>
@@ -2341,13 +2341,13 @@
     </row>
     <row r="65" spans="2:5">
       <c r="B65" s="6">
-        <v>5.31E-4</v>
+        <v>5.4100000000000003E-4</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>78</v>
       </c>
       <c r="D65" s="6">
-        <v>5.31E-4</v>
+        <v>5.4100000000000003E-4</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>198</v>
@@ -2355,13 +2355,13 @@
     </row>
     <row r="66" spans="2:5">
       <c r="B66" s="6">
-        <v>4.1510000000000002E-3</v>
+        <v>4.1939999999999998E-3</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>79</v>
       </c>
       <c r="D66" s="6">
-        <v>4.1510000000000002E-3</v>
+        <v>4.1939999999999998E-3</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>199</v>
@@ -2369,13 +2369,13 @@
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="6">
-        <v>7.4399999999999998E-4</v>
+        <v>7.4200000000000004E-4</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>80</v>
       </c>
       <c r="D67" s="6">
-        <v>7.4399999999999998E-4</v>
+        <v>7.4200000000000004E-4</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>200</v>
@@ -2397,13 +2397,13 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="6">
-        <v>1.8779999999999999E-3</v>
+        <v>1.879E-3</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>82</v>
       </c>
       <c r="D69" s="6">
-        <v>1.8779999999999999E-3</v>
+        <v>1.879E-3</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>202</v>
@@ -2411,13 +2411,13 @@
     </row>
     <row r="70" spans="2:5">
       <c r="B70" s="6">
-        <v>1.4729999999999999E-3</v>
+        <v>1.513E-3</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>83</v>
       </c>
       <c r="D70" s="6">
-        <v>1.4729999999999999E-3</v>
+        <v>1.513E-3</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>203</v>
@@ -2425,13 +2425,13 @@
     </row>
     <row r="71" spans="2:5">
       <c r="B71" s="6">
-        <v>5.829E-3</v>
+        <v>5.8650000000000004E-3</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>84</v>
       </c>
       <c r="D71" s="6">
-        <v>5.829E-3</v>
+        <v>5.8650000000000004E-3</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>204</v>
@@ -2439,13 +2439,13 @@
     </row>
     <row r="72" spans="2:5">
       <c r="B72" s="6">
-        <v>1.4404999999999999E-2</v>
+        <v>1.4533000000000001E-2</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>85</v>
       </c>
       <c r="D72" s="6">
-        <v>1.4404999999999999E-2</v>
+        <v>1.4533000000000001E-2</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>205</v>
@@ -2467,13 +2467,13 @@
     </row>
     <row r="74" spans="2:5">
       <c r="B74" s="6">
-        <v>3.4459999999999998E-3</v>
+        <v>3.4749999999999998E-3</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D74" s="6">
-        <v>3.4459999999999998E-3</v>
+        <v>3.4749999999999998E-3</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>207</v>
@@ -2481,13 +2481,13 @@
     </row>
     <row r="75" spans="2:5">
       <c r="B75" s="6">
-        <v>4.5511000000000003E-2</v>
+        <v>4.4595999999999997E-2</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>88</v>
       </c>
       <c r="D75" s="6">
-        <v>4.5511000000000003E-2</v>
+        <v>4.4595999999999997E-2</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>208</v>
@@ -2495,13 +2495,13 @@
     </row>
     <row r="76" spans="2:5">
       <c r="B76" s="6">
-        <v>8.4900000000000004E-4</v>
+        <v>8.5300000000000003E-4</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>89</v>
       </c>
       <c r="D76" s="6">
-        <v>8.4900000000000004E-4</v>
+        <v>8.5300000000000003E-4</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>209</v>
@@ -2509,13 +2509,13 @@
     </row>
     <row r="77" spans="2:5">
       <c r="B77" s="6">
-        <v>1.1299999999999999E-3</v>
+        <v>1.1529999999999999E-3</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>90</v>
       </c>
       <c r="D77" s="6">
-        <v>1.1299999999999999E-3</v>
+        <v>1.1529999999999999E-3</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>210</v>
@@ -2523,13 +2523,13 @@
     </row>
     <row r="78" spans="2:5">
       <c r="B78" s="6">
-        <v>4.0499999999999998E-4</v>
+        <v>4.0400000000000001E-4</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>91</v>
       </c>
       <c r="D78" s="6">
-        <v>4.0499999999999998E-4</v>
+        <v>4.0400000000000001E-4</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>211</v>
@@ -2551,13 +2551,13 @@
     </row>
     <row r="80" spans="2:5">
       <c r="B80" s="6">
-        <v>4.8929999999999998E-3</v>
+        <v>4.895E-3</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>93</v>
       </c>
       <c r="D80" s="6">
-        <v>4.8929999999999998E-3</v>
+        <v>4.895E-3</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>213</v>
@@ -2621,13 +2621,13 @@
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="6">
-        <v>5.4520000000000002E-3</v>
+        <v>5.4539999999999996E-3</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>98</v>
       </c>
       <c r="D85" s="6">
-        <v>5.4520000000000002E-3</v>
+        <v>5.4539999999999996E-3</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>218</v>
@@ -2677,13 +2677,13 @@
     </row>
     <row r="89" spans="2:5">
       <c r="B89" s="6">
-        <v>2.7179999999999999E-2</v>
+        <v>2.7193999999999999E-2</v>
       </c>
       <c r="C89" s="11" t="s">
         <v>102</v>
       </c>
       <c r="D89" s="6">
-        <v>2.7179999999999999E-2</v>
+        <v>2.7193999999999999E-2</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>222</v>
@@ -2691,13 +2691,13 @@
     </row>
     <row r="90" spans="2:5">
       <c r="B90" s="6">
-        <v>4.26E-4</v>
+        <v>4.2700000000000002E-4</v>
       </c>
       <c r="C90" s="11" t="s">
         <v>103</v>
       </c>
       <c r="D90" s="6">
-        <v>4.26E-4</v>
+        <v>4.2700000000000002E-4</v>
       </c>
       <c r="E90" s="11" t="s">
         <v>223</v>
@@ -2705,13 +2705,13 @@
     </row>
     <row r="91" spans="2:5">
       <c r="B91" s="6">
-        <v>2.6200000000000003E-4</v>
+        <v>2.63E-4</v>
       </c>
       <c r="C91" s="11" t="s">
         <v>104</v>
       </c>
       <c r="D91" s="6">
-        <v>2.6200000000000003E-4</v>
+        <v>2.63E-4</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>224</v>
@@ -2761,13 +2761,13 @@
     </row>
     <row r="95" spans="2:5">
       <c r="B95" s="6">
-        <v>8.3990000000000002E-3</v>
+        <v>8.4019999999999997E-3</v>
       </c>
       <c r="C95" s="11" t="s">
         <v>108</v>
       </c>
       <c r="D95" s="6">
-        <v>8.3990000000000002E-3</v>
+        <v>8.4019999999999997E-3</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>228</v>
@@ -2803,13 +2803,13 @@
     </row>
     <row r="98" spans="2:5">
       <c r="B98" s="6">
-        <v>1.8445E-2</v>
+        <v>1.8460000000000001E-2</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D98" s="6">
-        <v>1.8445E-2</v>
+        <v>1.8460000000000001E-2</v>
       </c>
       <c r="E98" s="11" t="s">
         <v>231</v>
@@ -2817,13 +2817,13 @@
     </row>
     <row r="99" spans="2:5">
       <c r="B99" s="6">
-        <v>7.4100000000000001E-4</v>
+        <v>7.4200000000000004E-4</v>
       </c>
       <c r="C99" s="11" t="s">
         <v>112</v>
       </c>
       <c r="D99" s="6">
-        <v>7.4100000000000001E-4</v>
+        <v>7.4200000000000004E-4</v>
       </c>
       <c r="E99" s="11" t="s">
         <v>232</v>
@@ -2831,13 +2831,13 @@
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="6">
-        <v>2.3519999999999999E-3</v>
+        <v>2.3570000000000002E-3</v>
       </c>
       <c r="C100" s="11" t="s">
         <v>113</v>
       </c>
       <c r="D100" s="6">
-        <v>2.3519999999999999E-3</v>
+        <v>2.3570000000000002E-3</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>233</v>
@@ -2845,13 +2845,13 @@
     </row>
     <row r="101" spans="2:5">
       <c r="B101" s="6">
-        <v>1.111E-3</v>
+        <v>1.1130000000000001E-3</v>
       </c>
       <c r="C101" s="11" t="s">
         <v>114</v>
       </c>
       <c r="D101" s="6">
-        <v>1.111E-3</v>
+        <v>1.1130000000000001E-3</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>234</v>
@@ -2873,13 +2873,13 @@
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="6">
-        <v>4.6439999999999997E-3</v>
+        <v>4.6449999999999998E-3</v>
       </c>
       <c r="C103" s="11" t="s">
         <v>116</v>
       </c>
       <c r="D103" s="6">
-        <v>4.6439999999999997E-3</v>
+        <v>4.6449999999999998E-3</v>
       </c>
       <c r="E103" s="11" t="s">
         <v>236</v>
@@ -2915,13 +2915,13 @@
     </row>
     <row r="106" spans="2:5">
       <c r="B106" s="6">
-        <v>7.6369999999999997E-3</v>
+        <v>7.7190000000000002E-3</v>
       </c>
       <c r="C106" s="11" t="s">
         <v>119</v>
       </c>
       <c r="D106" s="6">
-        <v>7.6369999999999997E-3</v>
+        <v>7.7190000000000002E-3</v>
       </c>
       <c r="E106" s="11" t="s">
         <v>239</v>
@@ -2929,13 +2929,13 @@
     </row>
     <row r="107" spans="2:5">
       <c r="B107" s="6">
-        <v>7.45E-4</v>
+        <v>7.4299999999999995E-4</v>
       </c>
       <c r="C107" s="11" t="s">
         <v>120</v>
       </c>
       <c r="D107" s="6">
-        <v>7.45E-4</v>
+        <v>7.4299999999999995E-4</v>
       </c>
       <c r="E107" s="11" t="s">
         <v>240</v>
@@ -2957,13 +2957,13 @@
     </row>
     <row r="109" spans="2:5">
       <c r="B109" s="6">
-        <v>2.8019999999999998E-3</v>
+        <v>2.8119999999999998E-3</v>
       </c>
       <c r="C109" s="11" t="s">
         <v>122</v>
       </c>
       <c r="D109" s="6">
-        <v>2.8019999999999998E-3</v>
+        <v>2.8119999999999998E-3</v>
       </c>
       <c r="E109" s="11" t="s">
         <v>242</v>
@@ -2971,13 +2971,13 @@
     </row>
     <row r="110" spans="2:5">
       <c r="B110" s="6">
-        <v>2.8419999999999999E-3</v>
+        <v>2.846E-3</v>
       </c>
       <c r="C110" s="11" t="s">
         <v>123</v>
       </c>
       <c r="D110" s="6">
-        <v>2.8419999999999999E-3</v>
+        <v>2.846E-3</v>
       </c>
       <c r="E110" s="11" t="s">
         <v>243</v>
@@ -2999,13 +2999,13 @@
     </row>
     <row r="112" spans="2:5">
       <c r="B112" s="6">
-        <v>3.6812999999999999E-2</v>
+        <v>3.6989000000000001E-2</v>
       </c>
       <c r="C112" s="11" t="s">
         <v>125</v>
       </c>
       <c r="D112" s="6">
-        <v>3.6812999999999999E-2</v>
+        <v>3.6989000000000001E-2</v>
       </c>
       <c r="E112" s="11" t="s">
         <v>245</v>
@@ -3027,13 +3027,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="B114" s="6">
-        <v>4.2729999999999999E-3</v>
+        <v>4.287E-3</v>
       </c>
       <c r="C114" s="11" t="s">
         <v>127</v>
       </c>
       <c r="D114" s="6">
-        <v>4.2729999999999999E-3</v>
+        <v>4.287E-3</v>
       </c>
       <c r="E114" s="11" t="s">
         <v>247</v>
@@ -3041,13 +3041,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="B115" s="6">
-        <v>3.6471999999999997E-2</v>
+        <v>3.3168999999999997E-2</v>
       </c>
       <c r="C115" s="11" t="s">
         <v>128</v>
       </c>
       <c r="D115" s="6">
-        <v>3.6471999999999997E-2</v>
+        <v>3.3168999999999997E-2</v>
       </c>
       <c r="E115" s="11" t="s">
         <v>248</v>
@@ -3055,13 +3055,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="B116" s="6">
-        <v>1.2149999999999999E-3</v>
+        <v>1.219E-3</v>
       </c>
       <c r="C116" s="11" t="s">
         <v>129</v>
       </c>
       <c r="D116" s="6">
-        <v>1.2149999999999999E-3</v>
+        <v>1.219E-3</v>
       </c>
       <c r="E116" s="11" t="s">
         <v>249</v>
@@ -3069,13 +3069,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="B117" s="6">
-        <v>2.3119999999999998E-3</v>
+        <v>2.313E-3</v>
       </c>
       <c r="C117" s="11" t="s">
         <v>130</v>
       </c>
       <c r="D117" s="6">
-        <v>2.3119999999999998E-3</v>
+        <v>2.313E-3</v>
       </c>
       <c r="E117" s="11" t="s">
         <v>250</v>
@@ -3111,13 +3111,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="B120" s="6">
-        <v>7.2760000000000003E-3</v>
+        <v>7.2779999999999997E-3</v>
       </c>
       <c r="C120" s="11" t="s">
         <v>133</v>
       </c>
       <c r="D120" s="6">
-        <v>7.2760000000000003E-3</v>
+        <v>7.2779999999999997E-3</v>
       </c>
       <c r="E120" s="11" t="s">
         <v>253</v>
@@ -3157,12 +3157,12 @@
       </c>
       <c r="B123" s="5">
         <f>AVERAGE(B3:B122)</f>
-        <v>8.6398916666666648E-3</v>
+        <v>8.6057250000000016E-3</v>
       </c>
       <c r="C123" s="13"/>
       <c r="D123" s="5">
         <f>AVERAGE(D3:D122)</f>
-        <v>8.6398916666666648E-3</v>
+        <v>8.6057250000000016E-3</v>
       </c>
       <c r="E123" s="13"/>
     </row>
@@ -3172,12 +3172,12 @@
       </c>
       <c r="B124" s="3">
         <f>MEDIAN(B3:B122)</f>
-        <v>4.5614999999999996E-3</v>
+        <v>4.5605000000000003E-3</v>
       </c>
       <c r="C124" s="10"/>
       <c r="D124" s="3">
         <f>MEDIAN(D3:D122)</f>
-        <v>4.5614999999999996E-3</v>
+        <v>4.5605000000000003E-3</v>
       </c>
       <c r="E124" s="10"/>
     </row>
@@ -3187,12 +3187,12 @@
       </c>
       <c r="B125" s="5">
         <f>AVERAGE(B3:B7,B12:B17,B21,B23:B26,B31,B34,B39:B47,B52:B57,B61,B63:B66,B71,B74,B79:B87,B92:B97,B101,B103:B106,B111,B114,B119:B122)</f>
-        <v>6.1087878787878802E-3</v>
+        <v>6.1122272727272744E-3</v>
       </c>
       <c r="C125" s="13"/>
       <c r="D125" s="5">
         <f>AVERAGE(D3:D7,D12:D17,D21,D23:D26,D31,D34,D39:D47,D52:D57,D61,D63:D66,D71,D74,D79:D87,D92:D97,D101,D103:D106,D111,D114,D119:D122)</f>
-        <v>6.1087878787878802E-3</v>
+        <v>6.1122272727272744E-3</v>
       </c>
       <c r="E125" s="13"/>
     </row>
@@ -3202,12 +3202,12 @@
       </c>
       <c r="B126" s="3">
         <f>MEDIAN(B3:B7,B12:B17,B21,B23:B26,B31,B34,B39:B47,B52:B57,B61,B63:B66,B71,B74,B79:B87,B92:B97,B101,B103:B106,B111,B114,B119:B122)</f>
-        <v>5.6404999999999997E-3</v>
+        <v>5.6474999999999997E-3</v>
       </c>
       <c r="C126" s="10"/>
       <c r="D126" s="3">
         <f>MEDIAN(D3:D7,D12:D17,D21,D23:D26,D31,D34,D39:D47,D52:D57,D61,D63:D66,D71,D74,D79:D87,D92:D97,D101,D103:D106,D111,D114,D119:D122)</f>
-        <v>5.6404999999999997E-3</v>
+        <v>5.6474999999999997E-3</v>
       </c>
       <c r="E126" s="10"/>
     </row>
@@ -3217,12 +3217,12 @@
       </c>
       <c r="B127" s="5">
         <f>AVERAGE(B8:B11,B18:B20,B22,B27:B30,B32:B33,B35:B38,B48:B51,B58:B60,B62,B67:B70,B72:B73,B75:B78,B88:B91,B98:B100,B102,B107:B110,B112:B113,B115:B118)</f>
-        <v>1.1733462962962966E-2</v>
+        <v>1.1653333333333342E-2</v>
       </c>
       <c r="C127" s="13"/>
       <c r="D127" s="5">
         <f>AVERAGE(D8:D11,D18:D20,D22,D27:D30,D32:D33,D35:D38,D48:D51,D58:D60,D62,D67:D70,D72:D73,D75:D78,D88:D91,D98:D100,D102,D107:D110,D112:D113,D115:D118)</f>
-        <v>1.1733462962962966E-2</v>
+        <v>1.1653333333333342E-2</v>
       </c>
       <c r="E127" s="13"/>
     </row>
@@ -3247,12 +3247,12 @@
       </c>
       <c r="B129" s="5">
         <f>AVERAGE(B43:B82)</f>
-        <v>7.5818499999999985E-3</v>
+        <v>7.5681249999999976E-3</v>
       </c>
       <c r="C129" s="13"/>
       <c r="D129" s="5">
         <f>AVERAGE(D43:D82)</f>
-        <v>7.5818499999999985E-3</v>
+        <v>7.5681249999999976E-3</v>
       </c>
       <c r="E129" s="13"/>
     </row>
@@ -3262,12 +3262,12 @@
       </c>
       <c r="B130" s="3">
         <f>MEDIAN(B43:B82)</f>
-        <v>4.3024999999999999E-3</v>
+        <v>4.3239999999999997E-3</v>
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="3">
         <f>MEDIAN(D43:D82)</f>
-        <v>4.3024999999999999E-3</v>
+        <v>4.3239999999999997E-3</v>
       </c>
       <c r="E130" s="10"/>
     </row>
@@ -3277,12 +3277,12 @@
       </c>
       <c r="B131" s="5">
         <f>AVERAGE(B83:B122)</f>
-        <v>9.3313249999999997E-3</v>
+        <v>9.2571500000000004E-3</v>
       </c>
       <c r="C131" s="13"/>
       <c r="D131" s="5">
         <f>AVERAGE(D83:D122)</f>
-        <v>9.3313249999999997E-3</v>
+        <v>9.2571500000000004E-3</v>
       </c>
       <c r="E131" s="13"/>
     </row>
@@ -3292,12 +3292,12 @@
       </c>
       <c r="B132" s="3">
         <f>MEDIAN(B83:B122)</f>
-        <v>4.4029999999999998E-3</v>
+        <v>4.4099999999999999E-3</v>
       </c>
       <c r="C132" s="10"/>
       <c r="D132" s="3">
         <f>MEDIAN(D83:D122)</f>
-        <v>4.4029999999999998E-3</v>
+        <v>4.4099999999999999E-3</v>
       </c>
       <c r="E132" s="10"/>
     </row>
@@ -3307,12 +3307,12 @@
       </c>
       <c r="B133" s="5">
         <f>AVERAGE(B3:B42)</f>
-        <v>9.0065000000000006E-3</v>
+        <v>8.9919000000000006E-3</v>
       </c>
       <c r="C133" s="13"/>
       <c r="D133" s="5">
         <f>AVERAGE(D3:D42)</f>
-        <v>9.0065000000000006E-3</v>
+        <v>8.9919000000000006E-3</v>
       </c>
       <c r="E133" s="13"/>
     </row>
@@ -3322,12 +3322,12 @@
       </c>
       <c r="B134" s="3">
         <f>MEDIAN(B3:B42)</f>
-        <v>5.8954999999999997E-3</v>
+        <v>5.8969999999999995E-3</v>
       </c>
       <c r="C134" s="10"/>
       <c r="D134" s="3">
         <f>MEDIAN(D3:D42)</f>
-        <v>5.8954999999999997E-3</v>
+        <v>5.8969999999999995E-3</v>
       </c>
       <c r="E134" s="10"/>
     </row>

</xml_diff>